<commit_message>
Excel student database upload
</commit_message>
<xml_diff>
--- a/app/studentdata/student_db.xlsx
+++ b/app/studentdata/student_db.xlsx
@@ -20,57 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">collegeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">programID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">departmentID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">streamID</t>
+    <t xml:space="preserve">first_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_Name</t>
   </si>
   <si>
     <t xml:space="preserve">student_Enrollment</t>
   </si>
   <si>
-    <t xml:space="preserve">first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middle_Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_Name</t>
+    <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">semester</t>
   </si>
   <si>
     <t xml:space="preserve">emailID</t>
   </si>
   <si>
-    <t xml:space="preserve">ICT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Tech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE</t>
+    <t xml:space="preserve">Umang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharma</t>
   </si>
   <si>
     <t xml:space="preserve">BDA</t>
   </si>
   <si>
-    <t xml:space="preserve">Umang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R.K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharma</t>
+    <t xml:space="preserve">umang.sharma.301299@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Kush</t>
@@ -79,16 +61,25 @@
     <t xml:space="preserve">Patel</t>
   </si>
   <si>
+    <t xml:space="preserve">kushkushalpatel@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raj</t>
   </si>
   <si>
     <t xml:space="preserve">Paltanwale</t>
   </si>
   <si>
+    <t xml:space="preserve">20rajpaltanwale@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gennady</t>
   </si>
   <si>
     <t xml:space="preserve">Korotkevich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tourist@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -190,24 +181,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="10" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -232,116 +224,101 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="I3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="D4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G3" s="0" t="s">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="D5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="umang.sharma.301299@gmail.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="kushkushalpatel@gmail.com"/>
+    <hyperlink ref="I3" r:id="rId3" display="kushkushalpatel@gmail.com"/>
+    <hyperlink ref="G4" r:id="rId4" display="20rajpaltanwale@gmail.com"/>
+    <hyperlink ref="G5" r:id="rId5" display="tourist@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>